<commit_message>
Update- code clean up - data clean up
</commit_message>
<xml_diff>
--- a/results/fa-optimal.xlsx
+++ b/results/fa-optimal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hichul\Desktop\2020-2021\Fall of 2020\Independent Study\water-accessibility\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hichul\Desktop\Independent Study\water-accessibility\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58166E8D-1975-4591-B2AD-4AEAAEBD0520}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06316917-7D24-428E-8481-8C55068C7453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3576" yWindow="2076" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimal-Factor" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="28">
   <si>
     <t>fm</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>7 FA</t>
   </si>
 </sst>
 </file>
@@ -691,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,6 +1628,108 @@
         <v>0.1082259</v>
       </c>
     </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" s="38"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="38"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B67" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C67" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D67" s="32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68" s="1"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" s="33"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="34"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B72" s="35"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="37"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="23"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="6"/>
+      <c r="D74" s="7"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="25"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>